<commit_message>
added full list of data in files
</commit_message>
<xml_diff>
--- a/data_in/translate_SMTYP.xlsx
+++ b/data_in/translate_SMTYP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\winfs-proj\data\proj\havgem\Mo-PROJEKTKATALOG\Uppdrag\HaV\Datavärdskapet_oceanografi_och_marinbiologi\2022\Städning\Translate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424861E2-B9A1-470A-8613-6755FEA7ED6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC3D19F-C2F5-4FCD-84E9-F7A3D82C26C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10050" windowHeight="3250" xr2:uid="{1A0B3E34-E74F-4EB7-997F-926D3A9788AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2740" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="309">
   <si>
     <t>CM</t>
   </si>
@@ -946,6 +946,12 @@
   </si>
   <si>
     <t>&lt;use_code&gt;</t>
+  </si>
+  <si>
+    <t>Kontrollera metodik!&lt;or&gt;rörhämtare.&lt;or&gt;Other&lt;or&gt;HAU</t>
+  </si>
+  <si>
+    <t>&lt;use_blank&gt;</t>
   </si>
 </sst>
 </file>
@@ -1328,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23198DC7-7ECB-44AE-9516-21530A2BB8E3}">
-  <dimension ref="A1:H107"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3301,6 +3307,17 @@
       </c>
       <c r="G107" s="7"/>
     </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A108" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="G108" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>